<commit_message>
Making some real progress on RMD implementation.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/Note_sheet_CH.xlsx
+++ b/raw-data-prep/raw_data/Note_sheet_CH.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhilgard\Documents\GitHub\vg-dissertation\raw-data-prep\raw_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="11310"/>
   </bookViews>
@@ -153,9 +158,6 @@
     <t>6:15PM</t>
   </si>
   <si>
-    <t xml:space="preserve">Mizzou's football quarterback. Good session. </t>
-  </si>
-  <si>
     <t>JH</t>
   </si>
   <si>
@@ -250,6 +252,9 @@
   </si>
   <si>
     <t>Game 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good session. </t>
   </si>
 </sst>
 </file>
@@ -299,6 +304,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -346,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,7 +389,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -590,11 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,31 +626,31 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
         <v>74</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>75</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>70</v>
       </c>
-      <c r="K1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>71</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>72</v>
       </c>
-      <c r="N1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>41554</v>
       </c>
@@ -685,7 +692,7 @@
       </c>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41554</v>
       </c>
@@ -726,7 +733,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>41555</v>
       </c>
@@ -770,7 +777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>41555</v>
       </c>
@@ -811,7 +818,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>41555</v>
       </c>
@@ -855,7 +862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>41555</v>
       </c>
@@ -934,13 +941,13 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>41555</v>
       </c>
@@ -984,7 +991,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>41556</v>
       </c>
@@ -1025,7 +1032,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>41556</v>
       </c>
@@ -1069,7 +1076,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>41557</v>
       </c>
@@ -1113,7 +1120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>41557</v>
       </c>
@@ -1154,7 +1161,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>41557</v>
       </c>
@@ -1198,7 +1205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>41557</v>
       </c>
@@ -1242,7 +1249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>41557</v>
       </c>
@@ -1324,13 +1331,13 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>41557</v>
       </c>
@@ -1374,7 +1381,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>41557</v>
       </c>
@@ -1418,7 +1425,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>41559</v>
       </c>
@@ -1462,7 +1469,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>41559</v>
       </c>
@@ -1506,7 +1513,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>41559</v>
       </c>
@@ -1550,7 +1557,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>41559</v>
       </c>
@@ -1594,7 +1601,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>41559</v>
       </c>
@@ -1638,7 +1645,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>41561</v>
       </c>
@@ -1682,7 +1689,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>41561</v>
       </c>
@@ -1723,7 +1730,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>41561</v>
       </c>
@@ -1764,10 +1771,10 @@
         <v>11</v>
       </c>
       <c r="N27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>41562</v>
       </c>
@@ -1775,7 +1782,7 @@
         <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D28">
         <v>71</v>
@@ -1808,10 +1815,10 @@
         <v>39</v>
       </c>
       <c r="N28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>41562</v>
       </c>
@@ -1852,10 +1859,10 @@
         <v>11</v>
       </c>
       <c r="N29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>41562</v>
       </c>
@@ -1863,7 +1870,7 @@
         <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D30">
         <v>73</v>
@@ -1896,10 +1903,10 @@
         <v>11</v>
       </c>
       <c r="N30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>41562</v>
       </c>
@@ -1940,10 +1947,10 @@
         <v>11</v>
       </c>
       <c r="N31" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>41563</v>
       </c>
@@ -1981,13 +1988,13 @@
         <v>60</v>
       </c>
       <c r="M32" t="s">
+        <v>49</v>
+      </c>
+      <c r="N32" t="s">
         <v>50</v>
       </c>
-      <c r="N32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>41563</v>
       </c>
@@ -2028,10 +2035,10 @@
         <v>11</v>
       </c>
       <c r="N33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>41563</v>
       </c>
@@ -2072,10 +2079,10 @@
         <v>39</v>
       </c>
       <c r="N34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>41563</v>
       </c>
@@ -2116,7 +2123,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>41564</v>
       </c>
@@ -2124,7 +2131,7 @@
         <v>20</v>
       </c>
       <c r="C36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D36">
         <v>78</v>
@@ -2157,10 +2164,10 @@
         <v>11</v>
       </c>
       <c r="N36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>41564</v>
       </c>
@@ -2168,7 +2175,7 @@
         <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D37">
         <v>80</v>
@@ -2201,10 +2208,10 @@
         <v>39</v>
       </c>
       <c r="N37" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>41564</v>
       </c>
@@ -2212,7 +2219,7 @@
         <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D38">
         <v>79</v>
@@ -2242,13 +2249,13 @@
         <v>0</v>
       </c>
       <c r="M38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>41568</v>
       </c>
@@ -2289,7 +2296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>41568</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>41568</v>
       </c>
@@ -2371,10 +2378,10 @@
         <v>39</v>
       </c>
       <c r="N41" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41568</v>
       </c>
@@ -2412,13 +2419,13 @@
         <v>106</v>
       </c>
       <c r="M42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N42" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41569</v>
       </c>
@@ -2462,7 +2469,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>41569</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41569</v>
       </c>
@@ -2547,7 +2554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>41570</v>
       </c>
@@ -2588,18 +2595,18 @@
         <v>11</v>
       </c>
       <c r="N46" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>41570</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C47" t="s">
         <v>61</v>
-      </c>
-      <c r="C47" t="s">
-        <v>62</v>
       </c>
       <c r="D47">
         <v>90</v>
@@ -2632,10 +2639,10 @@
         <v>11</v>
       </c>
       <c r="N47" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>41570</v>
       </c>
@@ -2676,7 +2683,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>41570</v>
       </c>
@@ -2717,7 +2724,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>41570</v>
       </c>
@@ -2755,13 +2762,13 @@
         <v>323</v>
       </c>
       <c r="M50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N50" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>41571</v>
       </c>
@@ -2769,7 +2776,7 @@
         <v>20</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D51">
         <v>93</v>
@@ -2802,18 +2809,18 @@
         <v>11</v>
       </c>
       <c r="N51" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>41571</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" t="s">
         <v>66</v>
-      </c>
-      <c r="C52" t="s">
-        <v>67</v>
       </c>
       <c r="D52">
         <v>94</v>
@@ -2846,18 +2853,11 @@
         <v>11</v>
       </c>
       <c r="N52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N52">
-    <filterColumn colId="12">
-      <filters>
-        <filter val="."/>
-        <filter val="No/Maybe"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:N52"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>